<commit_message>
age_range format to meddemog
0-64 - the other way was creating negatives and then I'd have to filter
</commit_message>
<xml_diff>
--- a/01 background/Analysis_Specifications.xlsx
+++ b/01 background/Analysis_Specifications.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DATA\HCPF_Data_files_SECURE\Kim\isp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\FHPC\DATA\HCPF_Data_files_SECURE\Kim\isp\isp_utilization\01 background\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C35E93-84FC-452D-80F9-488227D98F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2F1BA9-6B3F-4898-891B-D6E8761061C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A163DE94-6307-4150-BFFB-6B4CE85967AB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{A163DE94-6307-4150-BFFB-6B4CE85967AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Specs" sheetId="2" r:id="rId1"/>
     <sheet name="Measures" sheetId="1" r:id="rId2"/>
+    <sheet name="notes_qs_kw" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="95">
   <si>
     <t>HCPF data measures</t>
   </si>
@@ -235,13 +235,100 @@
   </si>
   <si>
     <t>School Based Health Centers</t>
+  </si>
+  <si>
+    <t>pcmp_loc_type_cd</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Pct</t>
+  </si>
+  <si>
+    <t>Cumulative Count</t>
+  </si>
+  <si>
+    <t>Clinic - Practitioner</t>
+  </si>
+  <si>
+    <t>Non-Physician Practitioner - Group</t>
+  </si>
+  <si>
+    <t>Physician</t>
+  </si>
+  <si>
+    <t>Indian Health Services - FQHC</t>
+  </si>
+  <si>
+    <t>Hospital - General</t>
+  </si>
+  <si>
+    <t>Clinic - Dental</t>
+  </si>
+  <si>
+    <t>Nurse Practitioner</t>
+  </si>
+  <si>
+    <t>PROV_TYP_CD medlong2</t>
+  </si>
+  <si>
+    <t>pcmp_orgTyp</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>FQHC</t>
+  </si>
+  <si>
+    <t>RHC</t>
+  </si>
+  <si>
+    <t>IHS</t>
+  </si>
+  <si>
+    <t>Dental</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>Cumulative Pct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01_getClients.sas </t>
+  </si>
+  <si>
+    <t>proc freq data medlong2 order=freq;</t>
+  </si>
+  <si>
+    <t>tables pcmp_loc_type_cd / out = pcmp_types_medlong;</t>
+  </si>
+  <si>
+    <t>run;</t>
+  </si>
+  <si>
+    <t>exclude here? Or do we exclude dental by something else?</t>
+  </si>
+  <si>
+    <t>Do 'others' look right?</t>
+  </si>
+  <si>
+    <t>Question: county variable from meddemog or enr_cnty from medlong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question: RCCO/RAE = 1? </t>
+  </si>
+  <si>
+    <t>Question: ManagedCare continuous - ask again - last time I asked, it was managedcare =0 for all but that was bc I had a filter on the set :(</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +342,32 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -264,9 +377,38 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFC1C1C1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFC1C1C1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFC1C1C1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFC1C1C1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -276,13 +418,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -294,6 +432,41 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -612,17 +785,17 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="90.26953125" customWidth="1"/>
-    <col min="3" max="3" width="72.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.21875" customWidth="1"/>
+    <col min="3" max="3" width="72.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -630,64 +803,64 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>42186</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="2">
         <v>44742</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31" x14ac:dyDescent="0.35">
-      <c r="B9" s="5" t="s">
+    <row r="9" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -695,12 +868,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>54</v>
       </c>
@@ -714,385 +887,328 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3A2D1E-A317-4F30-B849-FF99E3DED383}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" customWidth="1"/>
+    <col min="1" max="1" width="43.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3" t="s">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3" t="s">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3" t="s">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
-      <c r="B25" s="3" t="s">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
-      <c r="B26" s="3" t="s">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
-      <c r="B27" s="3" t="s">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D30" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D31" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D32" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>65</v>
       </c>
       <c r="D33" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D34" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E34" s="6"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B37" s="7" t="s">
+    <row r="37" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B37" s="5" t="s">
         <v>56</v>
       </c>
       <c r="D37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B38" s="7" t="s">
+    <row r="38" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B38" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B39" s="7" t="s">
+    <row r="39" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B39" s="5" t="s">
         <v>58</v>
       </c>
       <c r="D39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="B40" s="7" t="s">
+    <row r="40" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B40" s="5" t="s">
         <v>59</v>
       </c>
       <c r="D40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B41" s="7" t="s">
+    <row r="41" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B41" s="5" t="s">
         <v>60</v>
       </c>
       <c r="D41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="B42" s="7" t="s">
+    <row r="42" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B42" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D42" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B43" s="6" t="s">
+    <row r="43" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B43" s="4" t="s">
         <v>62</v>
       </c>
       <c r="D43" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B44" s="6" t="s">
+    <row r="44" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B44" s="4" t="s">
         <v>63</v>
       </c>
       <c r="D44" t="s">
@@ -1103,4 +1219,286 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ABD9E30-0E83-45D6-AD1B-69694A25E681}">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.77734375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" style="15" customWidth="1"/>
+    <col min="7" max="7" width="42.33203125" style="9" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="10">
+        <v>30925002</v>
+      </c>
+      <c r="C3" s="11">
+        <v>55.563669357999999</v>
+      </c>
+      <c r="D3" s="10">
+        <v>30925002</v>
+      </c>
+      <c r="E3" s="11">
+        <v>55.563669357999999</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="10">
+        <v>20778610</v>
+      </c>
+      <c r="C4" s="11">
+        <v>37.333411191000003</v>
+      </c>
+      <c r="D4" s="10">
+        <v>51703612</v>
+      </c>
+      <c r="E4" s="11">
+        <v>92.897080548999995</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="10">
+        <v>2193843</v>
+      </c>
+      <c r="C5" s="11">
+        <v>3.9417286723</v>
+      </c>
+      <c r="D5" s="10">
+        <v>53897455</v>
+      </c>
+      <c r="E5" s="11">
+        <v>96.838809221999995</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="10">
+        <v>1345622</v>
+      </c>
+      <c r="C6" s="11">
+        <v>2.4177103008</v>
+      </c>
+      <c r="D6" s="10">
+        <v>55243077</v>
+      </c>
+      <c r="E6" s="11">
+        <v>99.256519522999994</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="10">
+        <v>344260</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0.61853993780000005</v>
+      </c>
+      <c r="D7" s="10">
+        <v>55587337</v>
+      </c>
+      <c r="E7" s="11">
+        <v>99.875059460000003</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="10">
+        <v>61847</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.11112194139999999</v>
+      </c>
+      <c r="D8" s="10">
+        <v>55649184</v>
+      </c>
+      <c r="E8" s="11">
+        <v>99.986181402</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="10">
+        <v>4232</v>
+      </c>
+      <c r="C9" s="11">
+        <v>7.6037327E-3</v>
+      </c>
+      <c r="D9" s="10">
+        <v>55653416</v>
+      </c>
+      <c r="E9" s="11">
+        <v>99.993785134000007</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="10">
+        <v>3450</v>
+      </c>
+      <c r="C10" s="11">
+        <v>6.1986951000000002E-3</v>
+      </c>
+      <c r="D10" s="10">
+        <v>55656866</v>
+      </c>
+      <c r="E10" s="11">
+        <v>99.999983829000001</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="12">
+        <v>9</v>
+      </c>
+      <c r="C11" s="11">
+        <v>1.61705E-5</v>
+      </c>
+      <c r="D11" s="10">
+        <v>55656875</v>
+      </c>
+      <c r="E11" s="12">
+        <v>100</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>